<commit_message>
14.05.19 Today sales  Updated 12:00am
</commit_message>
<xml_diff>
--- a/May/Othes/Daily requisition analysis of Tulip -2, Bagha..xlsx
+++ b/May/Othes/Daily requisition analysis of Tulip -2, Bagha..xlsx
@@ -523,9 +523,6 @@
     <t xml:space="preserve"> Gold</t>
   </si>
   <si>
-    <t>12.05.19</t>
-  </si>
-  <si>
     <t>Black &amp; Black_blue</t>
   </si>
   <si>
@@ -536,6 +533,9 @@
   </si>
   <si>
     <t xml:space="preserve">Black </t>
+  </si>
+  <si>
+    <t>14.05.19</t>
   </si>
 </sst>
 </file>
@@ -1198,7 +1198,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E140" sqref="E140"/>
+      <selection pane="bottomRight" activeCell="J145" sqref="J145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21"/>
@@ -1243,7 +1243,7 @@
         <v>77</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="6" customFormat="1" ht="12.75">
@@ -1271,14 +1271,14 @@
         <v>779.95</v>
       </c>
       <c r="C5" s="11">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="D5" s="13">
         <f>C5*B5</f>
-        <v>15599</v>
+        <v>46797</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" hidden="1">
@@ -1405,20 +1405,22 @@
       </c>
       <c r="E13" s="11"/>
     </row>
-    <row r="14" spans="1:5" s="5" customFormat="1" ht="15" hidden="1">
+    <row r="14" spans="1:5" s="5" customFormat="1" ht="15">
       <c r="A14" s="14" t="s">
         <v>161</v>
       </c>
       <c r="B14" s="15">
         <v>1159.8900000000001</v>
       </c>
-      <c r="C14" s="11"/>
+      <c r="C14" s="11">
+        <v>100</v>
+      </c>
       <c r="D14" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>115989.00000000001</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>85</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" hidden="1">
@@ -1481,22 +1483,20 @@
         <v>166</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15">
+    <row r="19" spans="1:5" ht="15" hidden="1">
       <c r="A19" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B19" s="12">
         <v>975.4325</v>
       </c>
-      <c r="C19" s="11">
-        <v>10</v>
-      </c>
+      <c r="C19" s="11"/>
       <c r="D19" s="13">
         <f t="shared" si="0"/>
-        <v>9754.3250000000007</v>
+        <v>0</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="5" customFormat="1" ht="15" hidden="1">
@@ -1573,19 +1573,17 @@
       </c>
       <c r="E24" s="11"/>
     </row>
-    <row r="25" spans="1:5" s="5" customFormat="1" ht="15">
+    <row r="25" spans="1:5" s="5" customFormat="1" ht="15" hidden="1">
       <c r="A25" s="14" t="s">
         <v>4</v>
       </c>
       <c r="B25" s="15">
         <v>980.44500000000005</v>
       </c>
-      <c r="C25" s="11">
-        <v>15</v>
-      </c>
+      <c r="C25" s="11"/>
       <c r="D25" s="16">
         <f>C25*B25</f>
-        <v>14706.675000000001</v>
+        <v>0</v>
       </c>
       <c r="E25" s="14" t="s">
         <v>144</v>
@@ -1621,17 +1619,19 @@
         <v>141</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="5" customFormat="1" ht="15" hidden="1">
+    <row r="28" spans="1:5" s="5" customFormat="1" ht="15">
       <c r="A28" s="14" t="s">
         <v>157</v>
       </c>
       <c r="B28" s="15">
         <v>5607.99</v>
       </c>
-      <c r="C28" s="11"/>
+      <c r="C28" s="11">
+        <v>2</v>
+      </c>
       <c r="D28" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>11215.98</v>
       </c>
       <c r="E28" s="14" t="s">
         <v>85</v>
@@ -1797,19 +1797,17 @@
         <v>80</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15">
+    <row r="40" spans="1:5" ht="15" hidden="1">
       <c r="A40" s="11" t="s">
         <v>120</v>
       </c>
       <c r="B40" s="12">
         <v>2788.96</v>
       </c>
-      <c r="C40" s="11">
-        <v>2</v>
-      </c>
+      <c r="C40" s="11"/>
       <c r="D40" s="13">
         <f t="shared" si="0"/>
-        <v>5577.92</v>
+        <v>0</v>
       </c>
       <c r="E40" s="14" t="s">
         <v>146</v>
@@ -1957,22 +1955,20 @@
         <v>80</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="15">
+    <row r="50" spans="1:5" ht="15" hidden="1">
       <c r="A50" s="11" t="s">
         <v>132</v>
       </c>
       <c r="B50" s="12">
         <v>7309.23</v>
       </c>
-      <c r="C50" s="11">
-        <v>2</v>
-      </c>
+      <c r="C50" s="11"/>
       <c r="D50" s="13">
         <f t="shared" si="0"/>
-        <v>14618.46</v>
+        <v>0</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="15" hidden="1">
@@ -2227,11 +2223,11 @@
         <v>1024.56</v>
       </c>
       <c r="C67" s="11">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D67" s="13">
         <f>B67*C67</f>
-        <v>18442.079999999998</v>
+        <v>10245.599999999999</v>
       </c>
       <c r="E67" s="11" t="s">
         <v>85</v>
@@ -2357,22 +2353,20 @@
       </c>
       <c r="E75" s="11"/>
     </row>
-    <row r="76" spans="1:5" ht="15">
+    <row r="76" spans="1:5" ht="15" hidden="1">
       <c r="A76" s="11" t="s">
         <v>145</v>
       </c>
       <c r="B76" s="12">
         <v>1072.675</v>
       </c>
-      <c r="C76" s="11">
-        <v>35</v>
-      </c>
+      <c r="C76" s="11"/>
       <c r="D76" s="13">
         <f>C76*B76</f>
-        <v>37543.625</v>
+        <v>0</v>
       </c>
       <c r="E76" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="15" hidden="1">
@@ -2391,17 +2385,19 @@
         <v>85</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="15" hidden="1">
+    <row r="78" spans="1:5" ht="15">
       <c r="A78" s="11" t="s">
         <v>151</v>
       </c>
       <c r="B78" s="12">
         <v>1189.9675</v>
       </c>
-      <c r="C78" s="11"/>
+      <c r="C78" s="11">
+        <v>10</v>
+      </c>
       <c r="D78" s="13">
         <f>C78*B78</f>
-        <v>0</v>
+        <v>11899.674999999999</v>
       </c>
       <c r="E78" s="11" t="s">
         <v>144</v>
@@ -3296,11 +3292,11 @@
       <c r="B136" s="41"/>
       <c r="C136" s="19">
         <f>SUM(C5:C135)</f>
-        <v>102</v>
+        <v>182</v>
       </c>
       <c r="D136" s="20">
         <f>SUBTOTAL(9,D8:D135)</f>
-        <v>100643.08499999999</v>
+        <v>149350.255</v>
       </c>
       <c r="E136" s="19"/>
     </row>
@@ -3347,7 +3343,7 @@
         <v>72</v>
       </c>
       <c r="C141" s="32">
-        <v>100000</v>
+        <v>150000</v>
       </c>
       <c r="D141" s="11"/>
       <c r="E141" s="22"/>
@@ -3401,7 +3397,7 @@
       </c>
       <c r="C146" s="29">
         <f>SUM(C140:C145)</f>
-        <v>100000</v>
+        <v>150000</v>
       </c>
       <c r="D146" s="30"/>
       <c r="E146" s="22"/>

</xml_diff>

<commit_message>
22.05.19 Today Last Sales Updated
</commit_message>
<xml_diff>
--- a/May/Othes/Daily requisition analysis of Tulip -2, Bagha..xlsx
+++ b/May/Othes/Daily requisition analysis of Tulip -2, Bagha..xlsx
@@ -538,13 +538,13 @@
     <t>Dark_blue</t>
   </si>
   <si>
-    <t>21.05.19</t>
-  </si>
-  <si>
     <t>Black_Gold</t>
   </si>
   <si>
     <t>Black &amp; Dark_blue</t>
+  </si>
+  <si>
+    <t>22.05.19</t>
   </si>
 </sst>
 </file>
@@ -1207,7 +1207,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F142" sqref="F142"/>
+      <selection pane="bottomRight" activeCell="E146" sqref="E146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21"/>
@@ -1252,7 +1252,7 @@
         <v>77</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="6" customFormat="1" ht="12.75">
@@ -1390,11 +1390,11 @@
         <v>946.36</v>
       </c>
       <c r="C12" s="11">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D12" s="13">
         <f t="shared" si="0"/>
-        <v>18927.2</v>
+        <v>9463.6</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>85</v>
@@ -1474,19 +1474,17 @@
       </c>
       <c r="E17" s="11"/>
     </row>
-    <row r="18" spans="1:5" ht="15">
+    <row r="18" spans="1:5" ht="15" hidden="1">
       <c r="A18" s="11" t="s">
         <v>165</v>
       </c>
       <c r="B18" s="12">
         <v>1140.8499999999999</v>
       </c>
-      <c r="C18" s="11">
-        <v>10</v>
-      </c>
+      <c r="C18" s="11"/>
       <c r="D18" s="13">
         <f t="shared" si="0"/>
-        <v>11408.5</v>
+        <v>0</v>
       </c>
       <c r="E18" s="11" t="s">
         <v>85</v>
@@ -1582,22 +1580,20 @@
       </c>
       <c r="E24" s="11"/>
     </row>
-    <row r="25" spans="1:5" s="5" customFormat="1" ht="15">
+    <row r="25" spans="1:5" s="5" customFormat="1" ht="15" hidden="1">
       <c r="A25" s="14" t="s">
         <v>4</v>
       </c>
       <c r="B25" s="15">
         <v>980.44500000000005</v>
       </c>
-      <c r="C25" s="11">
-        <v>10</v>
-      </c>
+      <c r="C25" s="11"/>
       <c r="D25" s="16">
         <f>C25*B25</f>
-        <v>9804.4500000000007</v>
+        <v>0</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15" hidden="1">
@@ -2058,22 +2054,20 @@
       </c>
       <c r="E55" s="11"/>
     </row>
-    <row r="56" spans="1:5" ht="15">
+    <row r="56" spans="1:5" ht="15" hidden="1">
       <c r="A56" s="11" t="s">
         <v>132</v>
       </c>
       <c r="B56" s="31">
         <v>7309.2275</v>
       </c>
-      <c r="C56" s="11">
-        <v>2</v>
-      </c>
+      <c r="C56" s="11"/>
       <c r="D56" s="13">
         <f t="shared" si="0"/>
-        <v>14618.455</v>
+        <v>0</v>
       </c>
       <c r="E56" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="15" hidden="1">
@@ -2256,19 +2250,17 @@
       </c>
       <c r="E68" s="11"/>
     </row>
-    <row r="69" spans="1:5" ht="15">
+    <row r="69" spans="1:5" ht="15" hidden="1">
       <c r="A69" s="11" t="s">
         <v>164</v>
       </c>
       <c r="B69" s="12">
         <v>1092.7249999999999</v>
       </c>
-      <c r="C69" s="11">
-        <v>12</v>
-      </c>
+      <c r="C69" s="11"/>
       <c r="D69" s="13">
         <f t="shared" si="0"/>
-        <v>13112.699999999999</v>
+        <v>0</v>
       </c>
       <c r="E69" s="11" t="s">
         <v>172</v>
@@ -2304,17 +2296,19 @@
       </c>
       <c r="E71" s="11"/>
     </row>
-    <row r="72" spans="1:5" ht="15" hidden="1">
+    <row r="72" spans="1:5" ht="15">
       <c r="A72" s="11" t="s">
         <v>143</v>
       </c>
       <c r="B72" s="12">
         <v>1014.53</v>
       </c>
-      <c r="C72" s="11"/>
+      <c r="C72" s="11">
+        <v>20</v>
+      </c>
       <c r="D72" s="13">
         <f>B72*C72</f>
-        <v>0</v>
+        <v>20290.599999999999</v>
       </c>
       <c r="E72" s="11" t="s">
         <v>163</v>
@@ -2566,19 +2560,17 @@
         <v>80</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="15">
+    <row r="89" spans="1:5" ht="15" hidden="1">
       <c r="A89" s="11" t="s">
         <v>158</v>
       </c>
       <c r="B89" s="12">
         <v>5607.98</v>
       </c>
-      <c r="C89" s="11">
-        <v>15</v>
-      </c>
+      <c r="C89" s="11"/>
       <c r="D89" s="13">
         <f>C89*B89</f>
-        <v>84119.7</v>
+        <v>0</v>
       </c>
       <c r="E89" s="11" t="s">
         <v>80</v>
@@ -2856,19 +2848,17 @@
         <v>80</v>
       </c>
     </row>
-    <row r="108" spans="1:5" ht="15">
+    <row r="108" spans="1:5" ht="15" hidden="1">
       <c r="A108" s="11" t="s">
         <v>106</v>
       </c>
       <c r="B108" s="12">
         <v>4896.21</v>
       </c>
-      <c r="C108" s="11">
-        <v>2</v>
-      </c>
+      <c r="C108" s="11"/>
       <c r="D108" s="13">
         <f t="shared" si="3"/>
-        <v>9792.42</v>
+        <v>0</v>
       </c>
       <c r="E108" s="11" t="s">
         <v>80</v>
@@ -3094,19 +3084,17 @@
       </c>
       <c r="E122" s="11"/>
     </row>
-    <row r="123" spans="1:5" ht="15">
+    <row r="123" spans="1:5" ht="15" hidden="1">
       <c r="A123" s="11" t="s">
         <v>122</v>
       </c>
       <c r="B123" s="12">
         <v>4389.95</v>
       </c>
-      <c r="C123" s="11">
-        <v>2</v>
-      </c>
+      <c r="C123" s="11"/>
       <c r="D123" s="13">
         <f t="shared" si="3"/>
-        <v>8779.9</v>
+        <v>0</v>
       </c>
       <c r="E123" s="11" t="s">
         <v>166</v>
@@ -3309,11 +3297,11 @@
       <c r="B136" s="41"/>
       <c r="C136" s="19">
         <f>SUM(C5:C135)</f>
-        <v>73</v>
+        <v>30</v>
       </c>
       <c r="D136" s="20">
         <f>SUBTOTAL(9,D5:D135)</f>
-        <v>170563.32500000001</v>
+        <v>29754.199999999997</v>
       </c>
       <c r="E136" s="19"/>
     </row>
@@ -3360,7 +3348,7 @@
         <v>72</v>
       </c>
       <c r="C141" s="32">
-        <v>170000</v>
+        <v>30000</v>
       </c>
       <c r="D141" s="11"/>
       <c r="E141" s="22"/>
@@ -3414,7 +3402,7 @@
       </c>
       <c r="C146" s="29">
         <f>SUM(C140:C145)</f>
-        <v>170000</v>
+        <v>30000</v>
       </c>
       <c r="D146" s="30"/>
       <c r="E146" s="22"/>

</xml_diff>

<commit_message>
27.05.19 Today Sales Last Updated 10:23 PM
</commit_message>
<xml_diff>
--- a/May/Othes/Daily requisition analysis of Tulip -2, Bagha..xlsx
+++ b/May/Othes/Daily requisition analysis of Tulip -2, Bagha..xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="177">
   <si>
     <t>Model Name</t>
   </si>
@@ -97,9 +97,6 @@
     <t>L23</t>
   </si>
   <si>
-    <t>L24</t>
-  </si>
-  <si>
     <t>L26</t>
   </si>
   <si>
@@ -439,9 +436,6 @@
     <t>Daily Requisition for Tulip -2</t>
   </si>
   <si>
-    <t>Darkblue</t>
-  </si>
-  <si>
     <t>BL90</t>
   </si>
   <si>
@@ -535,15 +529,9 @@
     <t>Black &amp; Dark_blue</t>
   </si>
   <si>
-    <t>Black 60 /Blue 20</t>
-  </si>
-  <si>
     <t>Z15</t>
   </si>
   <si>
-    <t>26.05.19</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Dark_Blue</t>
   </si>
   <si>
@@ -551,6 +539,15 @@
   </si>
   <si>
     <t xml:space="preserve"> Black </t>
+  </si>
+  <si>
+    <t>27.05.19</t>
+  </si>
+  <si>
+    <t>L52</t>
+  </si>
+  <si>
+    <t>White_Red</t>
   </si>
 </sst>
 </file>
@@ -1210,10 +1207,10 @@
   <dimension ref="A1:I147"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C140" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F78" sqref="F78"/>
+      <selection pane="bottomRight" activeCell="D150" sqref="D150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21"/>
@@ -1228,7 +1225,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="6" customFormat="1" ht="12.75">
       <c r="A1" s="35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B1" s="36"/>
       <c r="C1" s="36"/>
@@ -1237,7 +1234,7 @@
     </row>
     <row r="2" spans="1:5" s="6" customFormat="1" ht="12.75">
       <c r="A2" s="38" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
@@ -1246,16 +1243,16 @@
     </row>
     <row r="3" spans="1:5" s="6" customFormat="1" ht="12.75">
       <c r="A3" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>174</v>
@@ -1266,32 +1263,34 @@
         <v>0</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C4" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="E4" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="E4" s="10" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15" hidden="1">
+    </row>
+    <row r="5" spans="1:5" ht="15">
       <c r="A5" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5" s="12">
         <v>779.95</v>
       </c>
-      <c r="C5" s="11"/>
+      <c r="C5" s="11">
+        <v>100</v>
+      </c>
       <c r="D5" s="13">
         <f>C5*B5</f>
-        <v>0</v>
+        <v>77995</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>172</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" hidden="1">
@@ -1310,41 +1309,43 @@
     </row>
     <row r="7" spans="1:5" ht="15">
       <c r="A7" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B7" s="12">
         <v>789.97</v>
       </c>
       <c r="C7" s="11">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D7" s="13">
         <f t="shared" si="0"/>
-        <v>7899.7000000000007</v>
+        <v>15799.400000000001</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15" hidden="1">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15">
       <c r="A8" s="11" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B8" s="12">
         <v>769.92</v>
       </c>
-      <c r="C8" s="11"/>
+      <c r="C8" s="11">
+        <v>20</v>
+      </c>
       <c r="D8" s="13">
         <f>B8*C8</f>
-        <v>0</v>
+        <v>15398.4</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" hidden="1">
       <c r="A9" s="11" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B9" s="12">
         <v>896.23500000000001</v>
@@ -1355,28 +1356,30 @@
         <v>0</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="15" hidden="1">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15">
       <c r="A10" s="11" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B10" s="12">
         <v>901.24749999999995</v>
       </c>
-      <c r="C10" s="11"/>
+      <c r="C10" s="11">
+        <v>13</v>
+      </c>
       <c r="D10" s="13">
         <f>B10*C10</f>
-        <v>0</v>
+        <v>11716.217499999999</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15">
       <c r="A11" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B11" s="12">
         <v>858.14</v>
@@ -1389,25 +1392,23 @@
         <v>17162.8</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="15">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15" hidden="1">
       <c r="A12" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B12" s="12">
         <v>946.36</v>
       </c>
-      <c r="C12" s="11">
-        <v>20</v>
-      </c>
+      <c r="C12" s="11"/>
       <c r="D12" s="13">
         <f t="shared" si="0"/>
-        <v>18927.2</v>
+        <v>0</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15" hidden="1">
@@ -1424,27 +1425,25 @@
       </c>
       <c r="E13" s="11"/>
     </row>
-    <row r="14" spans="1:5" s="5" customFormat="1" ht="15">
+    <row r="14" spans="1:5" s="5" customFormat="1" ht="15" hidden="1">
       <c r="A14" s="14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B14" s="15">
         <v>1159.8900000000001</v>
       </c>
-      <c r="C14" s="11">
-        <v>30</v>
-      </c>
+      <c r="C14" s="11"/>
       <c r="D14" s="16">
         <f t="shared" si="0"/>
-        <v>34796.700000000004</v>
+        <v>0</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" hidden="1">
       <c r="A15" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B15" s="12">
         <v>887.21</v>
@@ -1458,7 +1457,7 @@
     </row>
     <row r="16" spans="1:5" ht="15" hidden="1">
       <c r="A16" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B16" s="12">
         <v>868.17</v>
@@ -1469,7 +1468,7 @@
         <v>0</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15" hidden="1">
@@ -1488,7 +1487,7 @@
     </row>
     <row r="18" spans="1:5" ht="15">
       <c r="A18" s="11" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B18" s="12">
         <v>1140.8499999999999</v>
@@ -1501,7 +1500,7 @@
         <v>22817</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>79</v>
+        <v>143</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15" hidden="1">
@@ -1517,12 +1516,12 @@
         <v>0</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="5" customFormat="1" ht="15" hidden="1">
       <c r="A20" s="14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B20" s="15">
         <v>985.46</v>
@@ -1561,7 +1560,7 @@
         <v>0</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15" hidden="1">
@@ -1577,7 +1576,7 @@
         <v>0</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15" hidden="1">
@@ -1607,7 +1606,7 @@
         <v>0</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15" hidden="1">
@@ -1624,25 +1623,27 @@
       </c>
       <c r="E26" s="11"/>
     </row>
-    <row r="27" spans="1:5" s="5" customFormat="1" ht="15" hidden="1">
+    <row r="27" spans="1:5" s="5" customFormat="1" ht="15">
       <c r="A27" s="14" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B27" s="15">
         <v>936.34</v>
       </c>
-      <c r="C27" s="11"/>
+      <c r="C27" s="11">
+        <v>20</v>
+      </c>
       <c r="D27" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18726.8</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="5" customFormat="1" ht="15" hidden="1">
       <c r="A28" s="14" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B28" s="15">
         <v>5607.99</v>
@@ -1653,12 +1654,12 @@
         <v>0</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15" hidden="1">
       <c r="A29" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B29" s="12">
         <v>955.38</v>
@@ -1672,7 +1673,7 @@
     </row>
     <row r="30" spans="1:5" ht="15" hidden="1">
       <c r="A30" s="11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B30" s="12">
         <v>1014.53</v>
@@ -1700,7 +1701,7 @@
     </row>
     <row r="32" spans="1:5" s="5" customFormat="1" ht="15" hidden="1">
       <c r="A32" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B32" s="15">
         <v>1159.8900000000001</v>
@@ -1711,7 +1712,7 @@
         <v>0</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15" hidden="1">
@@ -1727,7 +1728,7 @@
         <v>0</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="15" hidden="1">
@@ -1813,12 +1814,12 @@
         <v>0</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="15" hidden="1">
       <c r="A40" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B40" s="12">
         <v>2788.96</v>
@@ -1829,7 +1830,7 @@
         <v>0</v>
       </c>
       <c r="E40" s="14" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="15" hidden="1">
@@ -1845,28 +1846,30 @@
         <v>0</v>
       </c>
       <c r="E41" s="11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="15" hidden="1">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="15">
       <c r="A42" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B42" s="12">
         <v>6397.96</v>
       </c>
-      <c r="C42" s="11"/>
+      <c r="C42" s="11">
+        <v>4</v>
+      </c>
       <c r="D42" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>25591.84</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="15" hidden="1">
       <c r="A43" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B43" s="12">
         <v>5158.87</v>
@@ -1877,7 +1880,7 @@
         <v>0</v>
       </c>
       <c r="E43" s="11" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="15" hidden="1">
@@ -1893,7 +1896,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="15" hidden="1">
@@ -1923,12 +1926,12 @@
         <v>0</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="15" hidden="1">
       <c r="A47" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B47" s="12">
         <v>7851.58</v>
@@ -1939,12 +1942,12 @@
         <v>0</v>
       </c>
       <c r="E47" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="15" hidden="1">
       <c r="A48" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B48" s="12">
         <v>7714.24</v>
@@ -1955,7 +1958,7 @@
         <v>0</v>
       </c>
       <c r="E48" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="15" hidden="1">
@@ -1971,30 +1974,28 @@
         <v>0</v>
       </c>
       <c r="E49" s="11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="15">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="15" hidden="1">
       <c r="A50" s="11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B50" s="12">
         <v>6369.89</v>
       </c>
-      <c r="C50" s="11">
-        <v>5</v>
-      </c>
+      <c r="C50" s="11"/>
       <c r="D50" s="13">
         <f t="shared" si="0"/>
-        <v>31849.45</v>
+        <v>0</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="15" hidden="1">
       <c r="A51" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B51" s="12">
         <v>8877.14</v>
@@ -2005,12 +2006,12 @@
         <v>0</v>
       </c>
       <c r="E51" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="15" hidden="1">
       <c r="A52" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B52" s="12">
         <v>8573.3799999999992</v>
@@ -2021,12 +2022,12 @@
         <v>0</v>
       </c>
       <c r="E52" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="15" hidden="1">
       <c r="A53" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B53" s="12">
         <v>8967.36</v>
@@ -2037,12 +2038,12 @@
         <v>0</v>
       </c>
       <c r="E53" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="15" hidden="1">
       <c r="A54" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B54" s="12">
         <v>9012.48</v>
@@ -2053,12 +2054,12 @@
         <v>0</v>
       </c>
       <c r="E54" s="11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="15" hidden="1">
       <c r="A55" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B55" s="12">
         <v>1199.9925000000001</v>
@@ -2072,7 +2073,7 @@
     </row>
     <row r="56" spans="1:5" ht="15" hidden="1">
       <c r="A56" s="11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B56" s="31">
         <v>7309.2275</v>
@@ -2083,12 +2084,12 @@
         <v>0</v>
       </c>
       <c r="E56" s="11" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="15" hidden="1">
       <c r="A57" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B57" s="12">
         <v>1423.55</v>
@@ -2102,7 +2103,7 @@
     </row>
     <row r="58" spans="1:5" ht="15" hidden="1">
       <c r="A58" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B58" s="12">
         <v>1435.58</v>
@@ -2116,7 +2117,7 @@
     </row>
     <row r="59" spans="1:5" ht="15" hidden="1">
       <c r="A59" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B59" s="12">
         <v>1551.87</v>
@@ -2130,7 +2131,7 @@
     </row>
     <row r="60" spans="1:5" ht="15" hidden="1">
       <c r="A60" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B60" s="12">
         <v>1695.2275</v>
@@ -2141,7 +2142,7 @@
         <v>0</v>
       </c>
       <c r="E60" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="15" hidden="1">
@@ -2160,7 +2161,7 @@
     </row>
     <row r="62" spans="1:5" ht="15" hidden="1">
       <c r="A62" s="11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B62" s="34">
         <v>1169.9175</v>
@@ -2171,12 +2172,12 @@
         <v>0</v>
       </c>
       <c r="E62" s="11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="15" hidden="1">
       <c r="A63" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B63" s="31">
         <v>4973.3999999999996</v>
@@ -2187,23 +2188,25 @@
         <v>0</v>
       </c>
       <c r="E63" s="11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="15" hidden="1">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="15">
       <c r="A64" s="11" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B64" s="33">
         <v>1053.6275000000001</v>
       </c>
-      <c r="C64" s="11"/>
+      <c r="C64" s="11">
+        <v>10</v>
+      </c>
       <c r="D64" s="13">
         <f>B64*C64</f>
-        <v>0</v>
+        <v>10536.275000000001</v>
       </c>
       <c r="E64" s="11" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="15" hidden="1">
@@ -2222,7 +2225,7 @@
     </row>
     <row r="66" spans="1:5" ht="15" hidden="1">
       <c r="A66" s="11" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B66" s="12">
         <v>1072.675</v>
@@ -2233,44 +2236,44 @@
         <v>0</v>
       </c>
       <c r="E66" s="11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" ht="15">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="15" hidden="1">
       <c r="A67" s="11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B67" s="12">
         <v>1024.56</v>
       </c>
-      <c r="C67" s="11">
-        <v>20</v>
-      </c>
+      <c r="C67" s="11"/>
       <c r="D67" s="13">
         <f>B67*C67</f>
-        <v>20491.199999999997</v>
+        <v>0</v>
       </c>
       <c r="E67" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="15" hidden="1">
       <c r="A68" s="11" t="s">
-        <v>26</v>
+        <v>175</v>
       </c>
       <c r="B68" s="12">
-        <v>1145.8575000000001</v>
+        <v>1077.6875</v>
       </c>
       <c r="C68" s="11"/>
       <c r="D68" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E68" s="11"/>
+      <c r="E68" s="11" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="69" spans="1:5" ht="15" hidden="1">
       <c r="A69" s="11" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B69" s="12">
         <v>1092.7249999999999</v>
@@ -2281,12 +2284,12 @@
         <v>0</v>
       </c>
       <c r="E69" s="11" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="15" hidden="1">
       <c r="A70" s="11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B70" s="31">
         <v>4165.3874999999998</v>
@@ -2297,12 +2300,12 @@
         <v>0</v>
       </c>
       <c r="E70" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="15" hidden="1">
       <c r="A71" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B71" s="12">
         <v>1174.93</v>
@@ -2316,7 +2319,7 @@
     </row>
     <row r="72" spans="1:5" ht="15" hidden="1">
       <c r="A72" s="11" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B72" s="12">
         <v>1014.53</v>
@@ -2327,12 +2330,12 @@
         <v>0</v>
       </c>
       <c r="E72" s="11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="15" hidden="1">
       <c r="A73" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B73" s="12">
         <v>1273.175</v>
@@ -2346,7 +2349,7 @@
     </row>
     <row r="74" spans="1:5" ht="15" hidden="1">
       <c r="A74" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B74" s="12">
         <v>1077.6875</v>
@@ -2357,12 +2360,12 @@
         <v>0</v>
       </c>
       <c r="E74" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="15" hidden="1">
       <c r="A75" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B75" s="12">
         <v>1101.75</v>
@@ -2376,7 +2379,7 @@
     </row>
     <row r="76" spans="1:5" ht="15" hidden="1">
       <c r="A76" s="11" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B76" s="12">
         <v>1072.675</v>
@@ -2387,12 +2390,12 @@
         <v>0</v>
       </c>
       <c r="E76" s="11" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="15" hidden="1">
       <c r="A77" s="11" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B77" s="12">
         <v>1297.2349999999999</v>
@@ -2403,12 +2406,12 @@
         <v>0</v>
       </c>
       <c r="E77" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="15">
       <c r="A78" s="11" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B78" s="12">
         <v>1189.9675</v>
@@ -2421,12 +2424,12 @@
         <v>23799.35</v>
       </c>
       <c r="E78" s="11" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="15" hidden="1">
       <c r="A79" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B79" s="12">
         <v>8150.3249999999998</v>
@@ -2440,7 +2443,7 @@
     </row>
     <row r="80" spans="1:5" ht="15" hidden="1">
       <c r="A80" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B80" s="12">
         <v>9067.6124999999993</v>
@@ -2454,7 +2457,7 @@
     </row>
     <row r="81" spans="1:5" ht="15" hidden="1">
       <c r="A81" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B81" s="12">
         <v>8565.36</v>
@@ -2465,12 +2468,12 @@
         <v>0</v>
       </c>
       <c r="E81" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="15" hidden="1">
       <c r="A82" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B82" s="12">
         <v>11854.5625</v>
@@ -2484,7 +2487,7 @@
     </row>
     <row r="83" spans="1:5" ht="15" hidden="1">
       <c r="A83" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B83" s="12">
         <v>10616.475</v>
@@ -2495,12 +2498,12 @@
         <v>0</v>
       </c>
       <c r="E83" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="15" hidden="1">
       <c r="A84" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B84" s="12">
         <v>12215.4625</v>
@@ -2511,12 +2514,12 @@
         <v>0</v>
       </c>
       <c r="E84" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="15" hidden="1">
       <c r="A85" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B85" s="12">
         <v>12691.65</v>
@@ -2527,12 +2530,12 @@
         <v>0</v>
       </c>
       <c r="E85" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="15" hidden="1">
       <c r="A86" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B86" s="12">
         <v>9097.6875</v>
@@ -2543,12 +2546,12 @@
         <v>0</v>
       </c>
       <c r="E86" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="15" hidden="1">
       <c r="A87" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B87" s="12">
         <v>10285.65</v>
@@ -2559,12 +2562,12 @@
         <v>0</v>
       </c>
       <c r="E87" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="15" hidden="1">
       <c r="A88" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B88" s="12">
         <v>6342.8175000000001</v>
@@ -2575,12 +2578,12 @@
         <v>0</v>
       </c>
       <c r="E88" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="15" hidden="1">
       <c r="A89" s="11" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B89" s="12">
         <v>5607.98</v>
@@ -2591,12 +2594,12 @@
         <v>0</v>
       </c>
       <c r="E89" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="15" hidden="1">
       <c r="A90" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B90" s="12">
         <v>17443.5</v>
@@ -2610,7 +2613,7 @@
     </row>
     <row r="91" spans="1:5" ht="15" hidden="1">
       <c r="A91" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B91" s="12">
         <v>13914.7</v>
@@ -2624,7 +2627,7 @@
     </row>
     <row r="92" spans="1:5" ht="15" hidden="1">
       <c r="A92" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B92" s="12">
         <v>10133.27</v>
@@ -2638,7 +2641,7 @@
     </row>
     <row r="93" spans="1:5" ht="15" hidden="1">
       <c r="A93" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B93" s="12">
         <v>23704.11</v>
@@ -2652,7 +2655,7 @@
     </row>
     <row r="94" spans="1:5" ht="15" hidden="1">
       <c r="A94" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B94" s="12">
         <v>1371.42</v>
@@ -2663,12 +2666,12 @@
         <v>0</v>
       </c>
       <c r="E94" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="15" hidden="1">
       <c r="A95" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B95" s="12">
         <v>1410.5174999999999</v>
@@ -2682,7 +2685,7 @@
     </row>
     <row r="96" spans="1:5" ht="15" hidden="1">
       <c r="A96" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B96" s="12">
         <v>1694.2249999999999</v>
@@ -2693,12 +2696,12 @@
         <v>0</v>
       </c>
       <c r="E96" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="15" hidden="1">
       <c r="A97" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B97" s="17">
         <v>1219.04</v>
@@ -2709,12 +2712,12 @@
         <v>0</v>
       </c>
       <c r="E97" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="15" hidden="1">
       <c r="A98" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B98" s="18">
         <v>1336.33</v>
@@ -2725,12 +2728,12 @@
         <v>0</v>
       </c>
       <c r="E98" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="15" hidden="1">
       <c r="A99" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B99" s="12">
         <v>1871.6675</v>
@@ -2744,7 +2747,7 @@
     </row>
     <row r="100" spans="1:5" ht="15" hidden="1">
       <c r="A100" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B100" s="12">
         <v>1854.625</v>
@@ -2758,7 +2761,7 @@
     </row>
     <row r="101" spans="1:5" ht="15" hidden="1">
       <c r="A101" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B101" s="12">
         <v>1446.6075000000001</v>
@@ -2772,7 +2775,7 @@
     </row>
     <row r="102" spans="1:5" ht="15" hidden="1">
       <c r="A102" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B102" s="12">
         <v>7586.92</v>
@@ -2783,12 +2786,12 @@
         <v>0</v>
       </c>
       <c r="E102" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="15" hidden="1">
       <c r="A103" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B103" s="12">
         <v>8641.5499999999993</v>
@@ -2799,12 +2802,12 @@
         <v>0</v>
       </c>
       <c r="E103" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="15" hidden="1">
       <c r="A104" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B104" s="12">
         <v>5183.9274999999998</v>
@@ -2815,12 +2818,12 @@
         <v>0</v>
       </c>
       <c r="E104" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="15" hidden="1">
       <c r="A105" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B105" s="12">
         <v>5455.6049999999996</v>
@@ -2831,12 +2834,12 @@
         <v>0</v>
       </c>
       <c r="E105" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="15" hidden="1">
       <c r="A106" s="11" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B106" s="12">
         <v>4526.2875000000004</v>
@@ -2847,12 +2850,12 @@
         <v>0</v>
       </c>
       <c r="E106" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="15" hidden="1">
       <c r="A107" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B107" s="12">
         <v>5510.74</v>
@@ -2863,28 +2866,30 @@
         <v>0</v>
       </c>
       <c r="E107" s="11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" ht="15" hidden="1">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="15">
       <c r="A108" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B108" s="12">
         <v>4896.21</v>
       </c>
-      <c r="C108" s="11"/>
+      <c r="C108" s="11">
+        <v>4</v>
+      </c>
       <c r="D108" s="13">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>19584.84</v>
       </c>
       <c r="E108" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="15" hidden="1">
       <c r="A109" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B109" s="12">
         <v>5150.8500000000004</v>
@@ -2895,12 +2900,12 @@
         <v>0</v>
       </c>
       <c r="E109" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="15" hidden="1">
       <c r="A110" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B110" s="12">
         <v>4973.3999999999996</v>
@@ -2911,12 +2916,12 @@
         <v>0</v>
       </c>
       <c r="E110" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="15" hidden="1">
       <c r="A111" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B111" s="12">
         <v>5423.53</v>
@@ -2927,12 +2932,12 @@
         <v>0</v>
       </c>
       <c r="E111" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="15" hidden="1">
       <c r="A112" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B112" s="12">
         <v>5940.82</v>
@@ -2943,12 +2948,12 @@
         <v>0</v>
       </c>
       <c r="E112" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="113" spans="1:5" ht="15" hidden="1">
       <c r="A113" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B113" s="12">
         <v>5257.11</v>
@@ -2959,12 +2964,12 @@
         <v>0</v>
       </c>
       <c r="E113" s="11" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="114" spans="1:5" ht="15" hidden="1">
       <c r="A114" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B114" s="12">
         <v>2900.2325000000001</v>
@@ -2975,12 +2980,12 @@
         <v>0</v>
       </c>
       <c r="E114" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="15" hidden="1">
       <c r="A115" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B115" s="12">
         <v>3143.84</v>
@@ -2991,12 +2996,12 @@
         <v>0</v>
       </c>
       <c r="E115" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="15" hidden="1">
       <c r="A116" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B116" s="12">
         <v>3518.7750000000001</v>
@@ -3010,7 +3015,7 @@
     </row>
     <row r="117" spans="1:5" ht="15" hidden="1">
       <c r="A117" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B117" s="12">
         <v>3556.87</v>
@@ -3021,12 +3026,12 @@
         <v>0</v>
       </c>
       <c r="E117" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="15" hidden="1">
       <c r="A118" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B118" s="12">
         <v>3471.66</v>
@@ -3037,12 +3042,12 @@
         <v>0</v>
       </c>
       <c r="E118" s="11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="15" hidden="1">
       <c r="A119" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B119" s="12">
         <v>3919.7750000000001</v>
@@ -3053,12 +3058,12 @@
         <v>0</v>
       </c>
       <c r="E119" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="15" hidden="1">
       <c r="A120" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B120" s="12">
         <v>4534.3074999999999</v>
@@ -3069,12 +3074,12 @@
         <v>0</v>
       </c>
       <c r="E120" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="15" hidden="1">
       <c r="A121" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B121" s="12">
         <v>3433.56</v>
@@ -3085,12 +3090,12 @@
         <v>0</v>
       </c>
       <c r="E121" s="11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="15" hidden="1">
       <c r="A122" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B122" s="12">
         <v>4476.1625000000004</v>
@@ -3104,25 +3109,25 @@
     </row>
     <row r="123" spans="1:5" ht="15">
       <c r="A123" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B123" s="12">
         <v>4389.95</v>
       </c>
       <c r="C123" s="11">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D123" s="13">
         <f t="shared" si="3"/>
-        <v>21949.75</v>
+        <v>26339.699999999997</v>
       </c>
       <c r="E123" s="11" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="15" hidden="1">
       <c r="A124" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B124" s="12">
         <v>5269.14</v>
@@ -3133,12 +3138,12 @@
         <v>0</v>
       </c>
       <c r="E124" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="15" hidden="1">
       <c r="A125" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B125" s="12">
         <v>5921.7674999999999</v>
@@ -3149,12 +3154,12 @@
         <v>0</v>
       </c>
       <c r="E125" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="12" hidden="1" customHeight="1">
       <c r="A126" s="11" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B126" s="12">
         <v>1170.92</v>
@@ -3165,12 +3170,12 @@
         <v>0</v>
       </c>
       <c r="E126" s="11" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="15" hidden="1">
       <c r="A127" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B127" s="12">
         <v>3934.8125</v>
@@ -3181,12 +3186,12 @@
         <v>0</v>
       </c>
       <c r="E127" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="15" hidden="1">
       <c r="A128" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B128" s="12">
         <v>4027.0425</v>
@@ -3197,12 +3202,12 @@
         <v>0</v>
       </c>
       <c r="E128" s="11" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="129" spans="1:9" ht="15" hidden="1">
       <c r="A129" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B129" s="12">
         <v>3892.71</v>
@@ -3213,12 +3218,12 @@
         <v>0</v>
       </c>
       <c r="E129" s="11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="130" spans="1:9" ht="15" hidden="1">
       <c r="A130" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B130" s="12">
         <v>4507.24</v>
@@ -3229,12 +3234,12 @@
         <v>0</v>
       </c>
       <c r="E130" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="131" spans="1:9" ht="15" hidden="1">
       <c r="A131" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B131" s="12">
         <v>4409</v>
@@ -3245,12 +3250,12 @@
         <v>0</v>
       </c>
       <c r="E131" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="132" spans="1:9" ht="15" hidden="1">
       <c r="A132" s="11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B132" s="12">
         <v>4165.3900000000003</v>
@@ -3261,12 +3266,12 @@
         <v>0</v>
       </c>
       <c r="E132" s="11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="133" spans="1:9" ht="15" hidden="1">
       <c r="A133" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B133" s="12">
         <v>4115.26</v>
@@ -3277,30 +3282,30 @@
         <v>0</v>
       </c>
       <c r="E133" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="134" spans="1:9" ht="15">
       <c r="A134" s="11" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B134" s="12">
         <v>8599.4500000000007</v>
       </c>
       <c r="C134" s="11">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D134" s="13">
         <f t="shared" si="3"/>
-        <v>85994.5</v>
+        <v>17198.900000000001</v>
       </c>
       <c r="E134" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="135" spans="1:9" ht="15" hidden="1">
       <c r="A135" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B135" s="12">
         <v>12310.7</v>
@@ -3311,21 +3316,21 @@
         <v>0</v>
       </c>
       <c r="E135" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="136" spans="1:9" s="2" customFormat="1" ht="15">
       <c r="A136" s="41" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B136" s="41"/>
       <c r="C136" s="19">
         <f>SUM(C5:C135)</f>
-        <v>160</v>
+        <v>259</v>
       </c>
       <c r="D136" s="20">
         <f>SUBTOTAL(9,D5:D135)</f>
-        <v>285687.65000000002</v>
+        <v>302666.52249999996</v>
       </c>
       <c r="E136" s="19"/>
     </row>
@@ -3335,7 +3340,7 @@
     <row r="138" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
       <c r="A138" s="21"/>
       <c r="B138" s="42" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C138" s="42"/>
       <c r="D138" s="42"/>
@@ -3344,13 +3349,13 @@
     <row r="139" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
       <c r="A139" s="23"/>
       <c r="B139" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C139" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="C139" s="24" t="s">
-        <v>69</v>
-      </c>
       <c r="D139" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E139" s="22"/>
       <c r="I139" s="25"/>
@@ -3358,7 +3363,7 @@
     <row r="140" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
       <c r="A140" s="26"/>
       <c r="B140" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C140" s="27">
         <v>0</v>
@@ -3369,10 +3374,10 @@
     <row r="141" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
       <c r="A141" s="26"/>
       <c r="B141" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C141" s="32">
-        <v>400000</v>
+        <v>180000</v>
       </c>
       <c r="D141" s="11"/>
       <c r="E141" s="22"/>
@@ -3380,7 +3385,7 @@
     <row r="142" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
       <c r="A142" s="26"/>
       <c r="B142" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C142" s="27">
         <v>0</v>
@@ -3391,7 +3396,7 @@
     <row r="143" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
       <c r="A143" s="26"/>
       <c r="B143" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C143" s="27"/>
       <c r="D143" s="11"/>
@@ -3400,7 +3405,7 @@
     <row r="144" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
       <c r="A144" s="26"/>
       <c r="B144" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C144" s="27">
         <v>0</v>
@@ -3411,7 +3416,7 @@
     <row r="145" spans="1:5" s="6" customFormat="1" ht="15.75" customHeight="1">
       <c r="A145" s="26"/>
       <c r="B145" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C145" s="27">
         <v>0</v>
@@ -3422,11 +3427,11 @@
     <row r="146" spans="1:5" s="6" customFormat="1" ht="15.75" customHeight="1">
       <c r="A146" s="23"/>
       <c r="B146" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C146" s="29">
         <f>SUM(C140:C145)</f>
-        <v>400000</v>
+        <v>180000</v>
       </c>
       <c r="D146" s="30"/>
       <c r="E146" s="22"/>

</xml_diff>

<commit_message>
30.05.19 Today Last Sales Updated 11:56 PM
</commit_message>
<xml_diff>
--- a/May/Othes/Daily requisition analysis of Tulip -2, Bagha..xlsx
+++ b/May/Othes/Daily requisition analysis of Tulip -2, Bagha..xlsx
@@ -10,14 +10,14 @@
     <sheet name="Daily Requisition" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Daily Requisition'!$A$4:$E$135</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Daily Requisition'!$A$4:$E$134</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="177">
   <si>
     <t>Model Name</t>
   </si>
@@ -466,9 +466,6 @@
     <t>Black_Green</t>
   </si>
   <si>
-    <t>Black &amp; Dark_Blue</t>
-  </si>
-  <si>
     <t>L90</t>
   </si>
   <si>
@@ -499,9 +496,6 @@
     <t>Black/Darkblue</t>
   </si>
   <si>
-    <t>L25i</t>
-  </si>
-  <si>
     <t>D54+</t>
   </si>
   <si>
@@ -535,18 +529,12 @@
     <t>Black &amp; Black_Red</t>
   </si>
   <si>
-    <t xml:space="preserve"> Black </t>
-  </si>
-  <si>
     <t>L52</t>
   </si>
   <si>
     <t>White_Red</t>
   </si>
   <si>
-    <t>28.05.19</t>
-  </si>
-  <si>
     <t>i72</t>
   </si>
   <si>
@@ -554,6 +542,12 @@
   </si>
   <si>
     <t xml:space="preserve"> Black &amp; Gold</t>
+  </si>
+  <si>
+    <t>30.05.19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gold &amp; Black </t>
   </si>
 </sst>
 </file>
@@ -1210,13 +1204,13 @@
   <sheetPr filterMode="1">
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:I147"/>
+  <dimension ref="A1:I146"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C140" sqref="C140"/>
+      <selection pane="bottomRight" activeCell="H137" sqref="H137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21"/>
@@ -1281,22 +1275,20 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15">
+    <row r="5" spans="1:5" ht="15" hidden="1">
       <c r="A5" s="11" t="s">
         <v>77</v>
       </c>
       <c r="B5" s="12">
         <v>779.95</v>
       </c>
-      <c r="C5" s="11">
-        <v>10</v>
-      </c>
+      <c r="C5" s="11"/>
       <c r="D5" s="13">
         <f>C5*B5</f>
-        <v>7799.5</v>
+        <v>0</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" hidden="1">
@@ -1308,7 +1300,7 @@
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="13">
-        <f t="shared" ref="D6:D95" si="0">C6*B6</f>
+        <f t="shared" ref="D6:D94" si="0">C6*B6</f>
         <v>0</v>
       </c>
       <c r="E6" s="11"/>
@@ -1326,7 +1318,7 @@
         <v>0</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" hidden="1">
@@ -1345,35 +1337,35 @@
         <v>140</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15" hidden="1">
+    <row r="9" spans="1:5" ht="15">
       <c r="A9" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B9" s="12">
         <v>896.23500000000001</v>
       </c>
-      <c r="C9" s="11"/>
+      <c r="C9" s="11">
+        <v>80</v>
+      </c>
       <c r="D9" s="13">
         <f>C9*B9</f>
-        <v>0</v>
+        <v>71698.8</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15">
+    <row r="10" spans="1:5" ht="15" hidden="1">
       <c r="A10" s="11" t="s">
         <v>138</v>
       </c>
       <c r="B10" s="12">
         <v>901.24749999999995</v>
       </c>
-      <c r="C10" s="11">
-        <v>20</v>
-      </c>
+      <c r="C10" s="11"/>
       <c r="D10" s="13">
         <f>B10*C10</f>
-        <v>18024.949999999997</v>
+        <v>0</v>
       </c>
       <c r="E10" s="11" t="s">
         <v>83</v>
@@ -1392,7 +1384,7 @@
         <v>0</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" hidden="1">
@@ -1408,7 +1400,7 @@
         <v>0</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15" hidden="1">
@@ -1425,19 +1417,17 @@
       </c>
       <c r="E13" s="11"/>
     </row>
-    <row r="14" spans="1:5" s="5" customFormat="1" ht="15">
+    <row r="14" spans="1:5" s="5" customFormat="1" ht="15" hidden="1">
       <c r="A14" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B14" s="15">
         <v>1159.8900000000001</v>
       </c>
-      <c r="C14" s="11">
-        <v>60</v>
-      </c>
+      <c r="C14" s="11"/>
       <c r="D14" s="16">
         <f t="shared" si="0"/>
-        <v>69593.400000000009</v>
+        <v>0</v>
       </c>
       <c r="E14" s="14" t="s">
         <v>83</v>
@@ -1455,9 +1445,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E15" s="11"/>
-    </row>
-    <row r="16" spans="1:5" ht="15" hidden="1">
+      <c r="E15" s="11" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" hidden="1">
       <c r="A16" s="11" t="s">
         <v>93</v>
       </c>
@@ -1468,9 +1460,6 @@
       <c r="D16" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15" hidden="1">
@@ -1487,22 +1476,20 @@
       </c>
       <c r="E17" s="11"/>
     </row>
-    <row r="18" spans="1:5" ht="15">
+    <row r="18" spans="1:5" ht="15" hidden="1">
       <c r="A18" s="11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B18" s="12">
         <v>1140.8499999999999</v>
       </c>
-      <c r="C18" s="11">
-        <v>80</v>
-      </c>
+      <c r="C18" s="11"/>
       <c r="D18" s="13">
         <f t="shared" si="0"/>
-        <v>91268</v>
+        <v>0</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15" hidden="1">
@@ -1518,7 +1505,7 @@
         <v>0</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="5" customFormat="1" ht="15" hidden="1">
@@ -1608,7 +1595,7 @@
         <v>0</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15" hidden="1">
@@ -1625,19 +1612,17 @@
       </c>
       <c r="E26" s="11"/>
     </row>
-    <row r="27" spans="1:5" s="5" customFormat="1" ht="15">
+    <row r="27" spans="1:5" s="5" customFormat="1" ht="15" hidden="1">
       <c r="A27" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B27" s="15">
         <v>936.34</v>
       </c>
-      <c r="C27" s="11">
-        <v>20</v>
-      </c>
+      <c r="C27" s="11"/>
       <c r="D27" s="16">
         <f t="shared" si="0"/>
-        <v>18726.8</v>
+        <v>0</v>
       </c>
       <c r="E27" s="14" t="s">
         <v>140</v>
@@ -1645,7 +1630,7 @@
     </row>
     <row r="28" spans="1:5" s="5" customFormat="1" ht="15" hidden="1">
       <c r="A28" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B28" s="15">
         <v>5607.99</v>
@@ -1701,19 +1686,17 @@
       </c>
       <c r="E31" s="11"/>
     </row>
-    <row r="32" spans="1:5" s="5" customFormat="1" ht="15">
+    <row r="32" spans="1:5" s="5" customFormat="1" ht="15" hidden="1">
       <c r="A32" s="14" t="s">
         <v>96</v>
       </c>
       <c r="B32" s="15">
         <v>1159.8900000000001</v>
       </c>
-      <c r="C32" s="11">
-        <v>10</v>
-      </c>
+      <c r="C32" s="11"/>
       <c r="D32" s="16">
         <f t="shared" si="0"/>
-        <v>11598.900000000001</v>
+        <v>0</v>
       </c>
       <c r="E32" s="14" t="s">
         <v>83</v>
@@ -1861,27 +1844,29 @@
         <v>6397.96</v>
       </c>
       <c r="C42" s="11">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D42" s="13">
         <f t="shared" si="0"/>
-        <v>31989.8</v>
+        <v>44785.72</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="15" hidden="1">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="15">
       <c r="A43" s="11" t="s">
         <v>104</v>
       </c>
       <c r="B43" s="12">
         <v>5158.87</v>
       </c>
-      <c r="C43" s="11"/>
+      <c r="C43" s="11">
+        <v>20</v>
+      </c>
       <c r="D43" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>103177.4</v>
       </c>
       <c r="E43" s="11" t="s">
         <v>142</v>
@@ -1933,22 +1918,20 @@
         <v>126</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15">
+    <row r="47" spans="1:5" ht="15" hidden="1">
       <c r="A47" s="11" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B47" s="12">
         <v>5793.45</v>
       </c>
-      <c r="C47" s="11">
-        <v>10</v>
-      </c>
+      <c r="C47" s="11"/>
       <c r="D47" s="13">
         <f t="shared" si="0"/>
-        <v>57934.5</v>
+        <v>0</v>
       </c>
       <c r="E47" s="11" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="15" hidden="1">
@@ -1991,14 +1974,14 @@
         <v>6369.89</v>
       </c>
       <c r="C50" s="11">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D50" s="13">
         <f t="shared" si="0"/>
-        <v>127397.8</v>
+        <v>95548.35</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="15" hidden="1">
@@ -2092,7 +2075,7 @@
         <v>0</v>
       </c>
       <c r="E56" s="11" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="15" hidden="1">
@@ -2167,35 +2150,35 @@
       </c>
       <c r="E61" s="11"/>
     </row>
-    <row r="62" spans="1:5" ht="15">
+    <row r="62" spans="1:5" ht="15" hidden="1">
       <c r="A62" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B62" s="34">
         <v>1169.9175</v>
       </c>
-      <c r="C62" s="11">
-        <v>10</v>
-      </c>
+      <c r="C62" s="11"/>
       <c r="D62" s="13">
         <f>B62*C62</f>
-        <v>11699.174999999999</v>
+        <v>0</v>
       </c>
       <c r="E62" s="11" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="15" hidden="1">
+    <row r="63" spans="1:5" ht="15">
       <c r="A63" s="11" t="s">
         <v>130</v>
       </c>
       <c r="B63" s="31">
         <v>4973.3999999999996</v>
       </c>
-      <c r="C63" s="11"/>
+      <c r="C63" s="11">
+        <v>3</v>
+      </c>
       <c r="D63" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>14920.199999999999</v>
       </c>
       <c r="E63" s="11" t="s">
         <v>78</v>
@@ -2233,7 +2216,7 @@
     </row>
     <row r="66" spans="1:5" ht="15" hidden="1">
       <c r="A66" s="11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B66" s="12">
         <v>1072.675</v>
@@ -2247,204 +2230,198 @@
         <v>83</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="15">
+    <row r="67" spans="1:5" ht="15" hidden="1">
       <c r="A67" s="11" t="s">
         <v>144</v>
       </c>
       <c r="B67" s="12">
         <v>1024.56</v>
       </c>
-      <c r="C67" s="11">
-        <v>20</v>
-      </c>
+      <c r="C67" s="11"/>
       <c r="D67" s="13">
         <f>B67*C67</f>
-        <v>20491.199999999997</v>
+        <v>0</v>
       </c>
       <c r="E67" s="11" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="15" hidden="1">
+    <row r="68" spans="1:5" ht="15">
       <c r="A68" s="11" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B68" s="12">
         <v>1077.6875</v>
       </c>
-      <c r="C68" s="11"/>
+      <c r="C68" s="11">
+        <v>20</v>
+      </c>
       <c r="D68" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>21553.75</v>
       </c>
       <c r="E68" s="11" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="15">
+    <row r="69" spans="1:5" ht="15" hidden="1">
       <c r="A69" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="B69" s="12">
-        <v>1092.7249999999999</v>
-      </c>
-      <c r="C69" s="11">
-        <v>30</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="B69" s="31">
+        <v>4165.3874999999998</v>
+      </c>
+      <c r="C69" s="11"/>
       <c r="D69" s="13">
         <f t="shared" si="0"/>
-        <v>32781.75</v>
+        <v>0</v>
       </c>
       <c r="E69" s="11" t="s">
-        <v>166</v>
+        <v>85</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="15" hidden="1">
       <c r="A70" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="B70" s="31">
-        <v>4165.3874999999998</v>
+        <v>26</v>
+      </c>
+      <c r="B70" s="12">
+        <v>1174.93</v>
       </c>
       <c r="C70" s="11"/>
       <c r="D70" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E70" s="11" t="s">
-        <v>85</v>
-      </c>
+      <c r="E70" s="11"/>
     </row>
     <row r="71" spans="1:5" ht="15" hidden="1">
       <c r="A71" s="11" t="s">
-        <v>26</v>
+        <v>139</v>
       </c>
       <c r="B71" s="12">
-        <v>1174.93</v>
+        <v>1014.53</v>
       </c>
       <c r="C71" s="11"/>
       <c r="D71" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E71" s="11"/>
-    </row>
-    <row r="72" spans="1:5" ht="15">
+        <f>B71*C71</f>
+        <v>0</v>
+      </c>
+      <c r="E71" s="11" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="15" hidden="1">
       <c r="A72" s="11" t="s">
-        <v>139</v>
+        <v>27</v>
       </c>
       <c r="B72" s="12">
-        <v>1014.53</v>
-      </c>
-      <c r="C72" s="11">
-        <v>80</v>
-      </c>
+        <v>1273.175</v>
+      </c>
+      <c r="C72" s="11"/>
       <c r="D72" s="13">
-        <f>B72*C72</f>
-        <v>81162.399999999994</v>
-      </c>
-      <c r="E72" s="11" t="s">
-        <v>159</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E72" s="11"/>
     </row>
     <row r="73" spans="1:5" ht="15" hidden="1">
       <c r="A73" s="11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B73" s="12">
-        <v>1273.175</v>
+        <v>1077.6875</v>
       </c>
       <c r="C73" s="11"/>
       <c r="D73" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E73" s="11"/>
+      <c r="E73" s="11" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="74" spans="1:5" ht="15" hidden="1">
       <c r="A74" s="11" t="s">
-        <v>28</v>
+        <v>97</v>
       </c>
       <c r="B74" s="12">
-        <v>1077.6875</v>
+        <v>1101.75</v>
       </c>
       <c r="C74" s="11"/>
       <c r="D74" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E74" s="11" t="s">
-        <v>85</v>
-      </c>
+      <c r="E74" s="11"/>
     </row>
     <row r="75" spans="1:5" ht="15" hidden="1">
       <c r="A75" s="11" t="s">
-        <v>97</v>
+        <v>141</v>
       </c>
       <c r="B75" s="12">
-        <v>1101.75</v>
+        <v>1072.675</v>
       </c>
       <c r="C75" s="11"/>
       <c r="D75" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E75" s="11"/>
+        <f>C75*B75</f>
+        <v>0</v>
+      </c>
+      <c r="E75" s="11" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="76" spans="1:5" ht="15" hidden="1">
       <c r="A76" s="11" t="s">
-        <v>141</v>
+        <v>155</v>
       </c>
       <c r="B76" s="12">
-        <v>1072.675</v>
+        <v>1297.2349999999999</v>
       </c>
       <c r="C76" s="11"/>
       <c r="D76" s="13">
-        <f>C76*B76</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E76" s="11" t="s">
-        <v>163</v>
+        <v>83</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="15" hidden="1">
       <c r="A77" s="11" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="B77" s="12">
-        <v>1297.2349999999999</v>
+        <v>1189.9675</v>
       </c>
       <c r="C77" s="11"/>
       <c r="D77" s="13">
-        <f t="shared" si="0"/>
+        <f>C77*B77</f>
         <v>0</v>
       </c>
       <c r="E77" s="11" t="s">
-        <v>83</v>
+        <v>164</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="15" hidden="1">
       <c r="A78" s="11" t="s">
-        <v>147</v>
+        <v>33</v>
       </c>
       <c r="B78" s="12">
-        <v>1189.9675</v>
+        <v>8150.3249999999998</v>
       </c>
       <c r="C78" s="11"/>
       <c r="D78" s="13">
-        <f>C78*B78</f>
-        <v>0</v>
-      </c>
-      <c r="E78" s="11" t="s">
-        <v>166</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E78" s="11"/>
     </row>
     <row r="79" spans="1:5" ht="15" hidden="1">
       <c r="A79" s="11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B79" s="12">
-        <v>8150.3249999999998</v>
+        <v>9067.6124999999993</v>
       </c>
       <c r="C79" s="11"/>
       <c r="D79" s="13">
@@ -2455,54 +2432,56 @@
     </row>
     <row r="80" spans="1:5" ht="15" hidden="1">
       <c r="A80" s="11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B80" s="12">
-        <v>9067.6124999999993</v>
+        <v>8565.36</v>
       </c>
       <c r="C80" s="11"/>
       <c r="D80" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E80" s="11"/>
+      <c r="E80" s="14" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="81" spans="1:5" ht="15" hidden="1">
       <c r="A81" s="11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B81" s="12">
-        <v>8565.36</v>
+        <v>11854.5625</v>
       </c>
       <c r="C81" s="11"/>
       <c r="D81" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E81" s="14" t="s">
-        <v>78</v>
-      </c>
+      <c r="E81" s="11"/>
     </row>
     <row r="82" spans="1:5" ht="15" hidden="1">
       <c r="A82" s="11" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B82" s="12">
-        <v>11854.5625</v>
+        <v>10616.475</v>
       </c>
       <c r="C82" s="11"/>
       <c r="D82" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E82" s="11"/>
+      <c r="E82" s="11" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="83" spans="1:5" ht="15" hidden="1">
       <c r="A83" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B83" s="12">
-        <v>10616.475</v>
+        <v>12215.4625</v>
       </c>
       <c r="C83" s="11"/>
       <c r="D83" s="13">
@@ -2510,15 +2489,15 @@
         <v>0</v>
       </c>
       <c r="E83" s="11" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="15" hidden="1">
       <c r="A84" s="11" t="s">
-        <v>37</v>
+        <v>82</v>
       </c>
       <c r="B84" s="12">
-        <v>12215.4625</v>
+        <v>12691.65</v>
       </c>
       <c r="C84" s="11"/>
       <c r="D84" s="13">
@@ -2526,15 +2505,15 @@
         <v>0</v>
       </c>
       <c r="E84" s="11" t="s">
-        <v>83</v>
+        <v>120</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="15" hidden="1">
       <c r="A85" s="11" t="s">
-        <v>82</v>
+        <v>40</v>
       </c>
       <c r="B85" s="12">
-        <v>12691.65</v>
+        <v>9097.6875</v>
       </c>
       <c r="C85" s="11"/>
       <c r="D85" s="13">
@@ -2542,15 +2521,15 @@
         <v>0</v>
       </c>
       <c r="E85" s="11" t="s">
-        <v>120</v>
+        <v>78</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="15" hidden="1">
       <c r="A86" s="11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B86" s="12">
-        <v>9097.6875</v>
+        <v>10285.65</v>
       </c>
       <c r="C86" s="11"/>
       <c r="D86" s="13">
@@ -2563,10 +2542,10 @@
     </row>
     <row r="87" spans="1:5" ht="15" hidden="1">
       <c r="A87" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B87" s="12">
-        <v>10285.65</v>
+        <v>6342.8175000000001</v>
       </c>
       <c r="C87" s="11"/>
       <c r="D87" s="13">
@@ -2579,44 +2558,40 @@
     </row>
     <row r="88" spans="1:5" ht="15" hidden="1">
       <c r="A88" s="11" t="s">
-        <v>39</v>
+        <v>153</v>
       </c>
       <c r="B88" s="12">
-        <v>6342.8175000000001</v>
+        <v>5607.98</v>
       </c>
       <c r="C88" s="11"/>
       <c r="D88" s="13">
-        <f t="shared" si="0"/>
+        <f>C88*B88</f>
         <v>0</v>
       </c>
       <c r="E88" s="11" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="15">
+    <row r="89" spans="1:5" ht="15" hidden="1">
       <c r="A89" s="11" t="s">
-        <v>154</v>
+        <v>109</v>
       </c>
       <c r="B89" s="12">
-        <v>5607.98</v>
-      </c>
-      <c r="C89" s="11">
-        <v>10</v>
-      </c>
+        <v>17443.5</v>
+      </c>
+      <c r="C89" s="11"/>
       <c r="D89" s="13">
-        <f>C89*B89</f>
-        <v>56079.799999999996</v>
-      </c>
-      <c r="E89" s="11" t="s">
-        <v>78</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E89" s="11"/>
     </row>
     <row r="90" spans="1:5" ht="15" hidden="1">
       <c r="A90" s="11" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B90" s="12">
-        <v>17443.5</v>
+        <v>13914.7</v>
       </c>
       <c r="C90" s="11"/>
       <c r="D90" s="13">
@@ -2627,98 +2602,100 @@
     </row>
     <row r="91" spans="1:5" ht="15" hidden="1">
       <c r="A91" s="11" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B91" s="12">
-        <v>13914.7</v>
+        <v>10133.27</v>
       </c>
       <c r="C91" s="11"/>
       <c r="D91" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D91" si="1">C91*B91</f>
         <v>0</v>
       </c>
       <c r="E91" s="11"/>
     </row>
     <row r="92" spans="1:5" ht="15" hidden="1">
       <c r="A92" s="11" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B92" s="12">
-        <v>10133.27</v>
+        <v>23704.11</v>
       </c>
       <c r="C92" s="11"/>
       <c r="D92" s="13">
-        <f t="shared" ref="D92" si="1">C92*B92</f>
+        <f t="shared" ref="D92" si="2">C92*B92</f>
         <v>0</v>
       </c>
       <c r="E92" s="11"/>
     </row>
     <row r="93" spans="1:5" ht="15" hidden="1">
       <c r="A93" s="11" t="s">
-        <v>108</v>
+        <v>42</v>
       </c>
       <c r="B93" s="12">
-        <v>23704.11</v>
+        <v>1371.42</v>
       </c>
       <c r="C93" s="11"/>
       <c r="D93" s="13">
-        <f t="shared" ref="D93" si="2">C93*B93</f>
-        <v>0</v>
-      </c>
-      <c r="E93" s="11"/>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E93" s="11" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="94" spans="1:5" ht="15" hidden="1">
       <c r="A94" s="11" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B94" s="12">
-        <v>1371.42</v>
+        <v>1410.5174999999999</v>
       </c>
       <c r="C94" s="11"/>
       <c r="D94" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E94" s="11" t="s">
-        <v>78</v>
-      </c>
+      <c r="E94" s="11"/>
     </row>
     <row r="95" spans="1:5" ht="15" hidden="1">
       <c r="A95" s="11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B95" s="12">
-        <v>1410.5174999999999</v>
+        <v>1694.2249999999999</v>
       </c>
       <c r="C95" s="11"/>
       <c r="D95" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E95" s="11"/>
+        <f t="shared" ref="D95:D134" si="3">C95*B95</f>
+        <v>0</v>
+      </c>
+      <c r="E95" s="11" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="96" spans="1:5" ht="15" hidden="1">
       <c r="A96" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B96" s="12">
-        <v>1694.2249999999999</v>
+        <v>116</v>
+      </c>
+      <c r="B96" s="17">
+        <v>1219.04</v>
       </c>
       <c r="C96" s="11"/>
       <c r="D96" s="13">
-        <f t="shared" ref="D96:D135" si="3">C96*B96</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E96" s="11" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="15" hidden="1">
       <c r="A97" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="B97" s="17">
-        <v>1219.04</v>
+        <v>121</v>
+      </c>
+      <c r="B97" s="18">
+        <v>1336.33</v>
       </c>
       <c r="C97" s="11"/>
       <c r="D97" s="13">
@@ -2731,26 +2708,24 @@
     </row>
     <row r="98" spans="1:5" ht="15" hidden="1">
       <c r="A98" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="B98" s="18">
-        <v>1336.33</v>
+        <v>46</v>
+      </c>
+      <c r="B98" s="12">
+        <v>1871.6675</v>
       </c>
       <c r="C98" s="11"/>
       <c r="D98" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E98" s="11" t="s">
-        <v>83</v>
-      </c>
+      <c r="E98" s="11"/>
     </row>
     <row r="99" spans="1:5" ht="15" hidden="1">
       <c r="A99" s="11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B99" s="12">
-        <v>1871.6675</v>
+        <v>1854.625</v>
       </c>
       <c r="C99" s="11"/>
       <c r="D99" s="13">
@@ -2761,10 +2736,10 @@
     </row>
     <row r="100" spans="1:5" ht="15" hidden="1">
       <c r="A100" s="11" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B100" s="12">
-        <v>1854.625</v>
+        <v>1446.6075000000001</v>
       </c>
       <c r="C100" s="11"/>
       <c r="D100" s="13">
@@ -2775,24 +2750,26 @@
     </row>
     <row r="101" spans="1:5" ht="15" hidden="1">
       <c r="A101" s="11" t="s">
-        <v>43</v>
+        <v>79</v>
       </c>
       <c r="B101" s="12">
-        <v>1446.6075000000001</v>
+        <v>7586.92</v>
       </c>
       <c r="C101" s="11"/>
       <c r="D101" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E101" s="11"/>
+      <c r="E101" s="11" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="102" spans="1:5" ht="15" hidden="1">
       <c r="A102" s="11" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B102" s="12">
-        <v>7586.92</v>
+        <v>8641.5499999999993</v>
       </c>
       <c r="C102" s="11"/>
       <c r="D102" s="13">
@@ -2805,10 +2782,10 @@
     </row>
     <row r="103" spans="1:5" ht="15" hidden="1">
       <c r="A103" s="11" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="B103" s="12">
-        <v>8641.5499999999993</v>
+        <v>5183.9274999999998</v>
       </c>
       <c r="C103" s="11"/>
       <c r="D103" s="13">
@@ -2816,15 +2793,15 @@
         <v>0</v>
       </c>
       <c r="E103" s="11" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="15" hidden="1">
       <c r="A104" s="11" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B104" s="12">
-        <v>5183.9274999999998</v>
+        <v>5455.6049999999996</v>
       </c>
       <c r="C104" s="11"/>
       <c r="D104" s="13">
@@ -2835,96 +2812,96 @@
         <v>78</v>
       </c>
     </row>
-    <row r="105" spans="1:5" ht="15" hidden="1">
+    <row r="105" spans="1:5" ht="15">
       <c r="A105" s="11" t="s">
-        <v>60</v>
+        <v>154</v>
       </c>
       <c r="B105" s="12">
-        <v>5455.6049999999996</v>
-      </c>
-      <c r="C105" s="11"/>
+        <v>4526.2875000000004</v>
+      </c>
+      <c r="C105" s="11">
+        <v>3</v>
+      </c>
       <c r="D105" s="13">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>C105*B105</f>
+        <v>13578.862500000001</v>
       </c>
       <c r="E105" s="11" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="15" hidden="1">
       <c r="A106" s="11" t="s">
-        <v>155</v>
+        <v>84</v>
       </c>
       <c r="B106" s="12">
-        <v>4526.2875000000004</v>
+        <v>5510.74</v>
       </c>
       <c r="C106" s="11"/>
       <c r="D106" s="13">
-        <f>C106*B106</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E106" s="11" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" ht="15" hidden="1">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="15">
       <c r="A107" s="11" t="s">
-        <v>84</v>
+        <v>103</v>
       </c>
       <c r="B107" s="12">
-        <v>5510.74</v>
-      </c>
-      <c r="C107" s="11"/>
+        <v>4896.21</v>
+      </c>
+      <c r="C107" s="11">
+        <v>10</v>
+      </c>
       <c r="D107" s="13">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>48962.1</v>
       </c>
       <c r="E107" s="11" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="108" spans="1:5" ht="15">
+    <row r="108" spans="1:5" ht="15" hidden="1">
       <c r="A108" s="11" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B108" s="12">
-        <v>4896.21</v>
-      </c>
-      <c r="C108" s="11">
-        <v>7</v>
-      </c>
+        <v>5150.8500000000004</v>
+      </c>
+      <c r="C108" s="11"/>
       <c r="D108" s="13">
         <f t="shared" si="3"/>
-        <v>34273.47</v>
+        <v>0</v>
       </c>
       <c r="E108" s="11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" ht="15">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="15" hidden="1">
       <c r="A109" s="11" t="s">
-        <v>98</v>
+        <v>130</v>
       </c>
       <c r="B109" s="12">
-        <v>5150.8500000000004</v>
-      </c>
-      <c r="C109" s="11">
-        <v>6</v>
-      </c>
+        <v>4973.3999999999996</v>
+      </c>
+      <c r="C109" s="11"/>
       <c r="D109" s="13">
         <f t="shared" si="3"/>
-        <v>30905.100000000002</v>
+        <v>0</v>
       </c>
       <c r="E109" s="11" t="s">
-        <v>127</v>
+        <v>78</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="15" hidden="1">
       <c r="A110" s="11" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="B110" s="12">
-        <v>4973.3999999999996</v>
+        <v>5423.53</v>
       </c>
       <c r="C110" s="11"/>
       <c r="D110" s="13">
@@ -2937,60 +2914,60 @@
     </row>
     <row r="111" spans="1:5" ht="15" hidden="1">
       <c r="A111" s="11" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B111" s="12">
-        <v>5423.53</v>
+        <v>5940.82</v>
       </c>
       <c r="C111" s="11"/>
       <c r="D111" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="D111" si="4">C111*B111</f>
         <v>0</v>
       </c>
       <c r="E111" s="11" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="112" spans="1:5" ht="15" hidden="1">
+    <row r="112" spans="1:5" ht="15">
       <c r="A112" s="11" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="B112" s="12">
-        <v>5940.82</v>
-      </c>
-      <c r="C112" s="11"/>
+        <v>5257.11</v>
+      </c>
+      <c r="C112" s="11">
+        <v>10</v>
+      </c>
       <c r="D112" s="13">
-        <f t="shared" ref="D112" si="4">C112*B112</f>
-        <v>0</v>
+        <f>C112*B112</f>
+        <v>52571.1</v>
       </c>
       <c r="E112" s="11" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="15" hidden="1">
+      <c r="A113" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B113" s="12">
+        <v>2900.2325000000001</v>
+      </c>
+      <c r="C113" s="11"/>
+      <c r="D113" s="13">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E113" s="11" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" ht="15">
-      <c r="A113" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="B113" s="12">
-        <v>5257.11</v>
-      </c>
-      <c r="C113" s="11">
-        <v>20</v>
-      </c>
-      <c r="D113" s="13">
-        <f>C113*B113</f>
-        <v>105142.2</v>
-      </c>
-      <c r="E113" s="11" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="114" spans="1:5" ht="15" hidden="1">
       <c r="A114" s="11" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B114" s="12">
-        <v>2900.2325000000001</v>
+        <v>3143.84</v>
       </c>
       <c r="C114" s="11"/>
       <c r="D114" s="13">
@@ -2998,45 +2975,45 @@
         <v>0</v>
       </c>
       <c r="E114" s="11" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="15" hidden="1">
       <c r="A115" s="11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B115" s="12">
-        <v>3143.84</v>
+        <v>3518.7750000000001</v>
       </c>
       <c r="C115" s="11"/>
       <c r="D115" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E115" s="11" t="s">
-        <v>83</v>
-      </c>
+      <c r="E115" s="11"/>
     </row>
     <row r="116" spans="1:5" ht="15" hidden="1">
       <c r="A116" s="11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B116" s="12">
-        <v>3518.7750000000001</v>
+        <v>3556.87</v>
       </c>
       <c r="C116" s="11"/>
       <c r="D116" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E116" s="11"/>
+      <c r="E116" s="11" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="117" spans="1:5" ht="15" hidden="1">
       <c r="A117" s="11" t="s">
-        <v>51</v>
+        <v>102</v>
       </c>
       <c r="B117" s="12">
-        <v>3556.87</v>
+        <v>3471.66</v>
       </c>
       <c r="C117" s="11"/>
       <c r="D117" s="13">
@@ -3044,15 +3021,15 @@
         <v>0</v>
       </c>
       <c r="E117" s="11" t="s">
-        <v>81</v>
+        <v>134</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="15" hidden="1">
       <c r="A118" s="11" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="B118" s="12">
-        <v>3471.66</v>
+        <v>3919.7750000000001</v>
       </c>
       <c r="C118" s="11"/>
       <c r="D118" s="13">
@@ -3060,15 +3037,15 @@
         <v>0</v>
       </c>
       <c r="E118" s="11" t="s">
-        <v>134</v>
+        <v>78</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="15" hidden="1">
       <c r="A119" s="11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B119" s="12">
-        <v>3919.7750000000001</v>
+        <v>4534.3074999999999</v>
       </c>
       <c r="C119" s="11"/>
       <c r="D119" s="13">
@@ -3081,10 +3058,10 @@
     </row>
     <row r="120" spans="1:5" ht="15" hidden="1">
       <c r="A120" s="11" t="s">
-        <v>53</v>
+        <v>124</v>
       </c>
       <c r="B120" s="12">
-        <v>4534.3074999999999</v>
+        <v>3433.56</v>
       </c>
       <c r="C120" s="11"/>
       <c r="D120" s="13">
@@ -3092,63 +3069,63 @@
         <v>0</v>
       </c>
       <c r="E120" s="11" t="s">
-        <v>78</v>
+        <v>131</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="15" hidden="1">
       <c r="A121" s="11" t="s">
-        <v>124</v>
+        <v>54</v>
       </c>
       <c r="B121" s="12">
-        <v>3433.56</v>
+        <v>4476.1625000000004</v>
       </c>
       <c r="C121" s="11"/>
       <c r="D121" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E121" s="11" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" ht="15" hidden="1">
+      <c r="E121" s="11"/>
+    </row>
+    <row r="122" spans="1:5" ht="15">
       <c r="A122" s="11" t="s">
-        <v>54</v>
+        <v>119</v>
       </c>
       <c r="B122" s="12">
-        <v>4476.1625000000004</v>
-      </c>
-      <c r="C122" s="11"/>
+        <v>4389.95</v>
+      </c>
+      <c r="C122" s="11">
+        <v>5</v>
+      </c>
       <c r="D122" s="13">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E122" s="11"/>
-    </row>
-    <row r="123" spans="1:5" ht="15">
+        <v>21949.75</v>
+      </c>
+      <c r="E122" s="11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" ht="15" hidden="1">
       <c r="A123" s="11" t="s">
-        <v>119</v>
+        <v>55</v>
       </c>
       <c r="B123" s="12">
-        <v>4389.95</v>
-      </c>
-      <c r="C123" s="11">
-        <v>40</v>
-      </c>
+        <v>5269.14</v>
+      </c>
+      <c r="C123" s="11"/>
       <c r="D123" s="13">
         <f t="shared" si="3"/>
-        <v>175598</v>
+        <v>0</v>
       </c>
       <c r="E123" s="11" t="s">
-        <v>162</v>
+        <v>78</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="15" hidden="1">
       <c r="A124" s="11" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B124" s="12">
-        <v>5269.14</v>
+        <v>5921.7674999999999</v>
       </c>
       <c r="C124" s="11"/>
       <c r="D124" s="13">
@@ -3159,44 +3136,44 @@
         <v>78</v>
       </c>
     </row>
-    <row r="125" spans="1:5" ht="15" hidden="1">
+    <row r="125" spans="1:5" ht="12" hidden="1" customHeight="1">
       <c r="A125" s="11" t="s">
-        <v>56</v>
+        <v>145</v>
       </c>
       <c r="B125" s="12">
-        <v>5921.7674999999999</v>
+        <v>1170.92</v>
       </c>
       <c r="C125" s="11"/>
       <c r="D125" s="13">
-        <f t="shared" si="3"/>
+        <f>C125*B125</f>
         <v>0</v>
       </c>
       <c r="E125" s="11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" ht="12" hidden="1" customHeight="1">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" ht="15" hidden="1">
       <c r="A126" s="11" t="s">
-        <v>145</v>
+        <v>57</v>
       </c>
       <c r="B126" s="12">
-        <v>1170.92</v>
+        <v>3934.8125</v>
       </c>
       <c r="C126" s="11"/>
       <c r="D126" s="13">
-        <f>C126*B126</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E126" s="11" t="s">
-        <v>165</v>
+        <v>78</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="15" hidden="1">
       <c r="A127" s="11" t="s">
-        <v>57</v>
+        <v>99</v>
       </c>
       <c r="B127" s="12">
-        <v>3934.8125</v>
+        <v>4027.0425</v>
       </c>
       <c r="C127" s="11"/>
       <c r="D127" s="13">
@@ -3204,33 +3181,31 @@
         <v>0</v>
       </c>
       <c r="E127" s="11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" ht="15">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" ht="15" hidden="1">
       <c r="A128" s="11" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="B128" s="12">
-        <v>4027.0425</v>
-      </c>
-      <c r="C128" s="11">
-        <v>3</v>
-      </c>
+        <v>3892.71</v>
+      </c>
+      <c r="C128" s="11"/>
       <c r="D128" s="13">
         <f t="shared" si="3"/>
-        <v>12081.127500000001</v>
+        <v>0</v>
       </c>
       <c r="E128" s="11" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
     </row>
     <row r="129" spans="1:9" ht="15" hidden="1">
       <c r="A129" s="11" t="s">
-        <v>118</v>
+        <v>58</v>
       </c>
       <c r="B129" s="12">
-        <v>3892.71</v>
+        <v>4507.24</v>
       </c>
       <c r="C129" s="11"/>
       <c r="D129" s="13">
@@ -3238,15 +3213,15 @@
         <v>0</v>
       </c>
       <c r="E129" s="11" t="s">
-        <v>134</v>
+        <v>78</v>
       </c>
     </row>
     <row r="130" spans="1:9" ht="15" hidden="1">
       <c r="A130" s="11" t="s">
-        <v>58</v>
+        <v>100</v>
       </c>
       <c r="B130" s="12">
-        <v>4507.24</v>
+        <v>4409</v>
       </c>
       <c r="C130" s="11"/>
       <c r="D130" s="13">
@@ -3259,10 +3234,10 @@
     </row>
     <row r="131" spans="1:9" ht="15" hidden="1">
       <c r="A131" s="11" t="s">
-        <v>100</v>
+        <v>128</v>
       </c>
       <c r="B131" s="12">
-        <v>4409</v>
+        <v>4165.3900000000003</v>
       </c>
       <c r="C131" s="11"/>
       <c r="D131" s="13">
@@ -3270,49 +3245,49 @@
         <v>0</v>
       </c>
       <c r="E131" s="11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="132" spans="1:9" ht="15" hidden="1">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" ht="15">
       <c r="A132" s="11" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="B132" s="12">
-        <v>4165.3900000000003</v>
-      </c>
-      <c r="C132" s="11"/>
+        <v>4115.26</v>
+      </c>
+      <c r="C132" s="11">
+        <v>4</v>
+      </c>
       <c r="D132" s="13">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>16461.04</v>
       </c>
       <c r="E132" s="11" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="133" spans="1:9" ht="15">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" ht="15" hidden="1">
       <c r="A133" s="11" t="s">
-        <v>112</v>
+        <v>167</v>
       </c>
       <c r="B133" s="12">
-        <v>4115.26</v>
-      </c>
-      <c r="C133" s="11">
-        <v>3</v>
-      </c>
+        <v>8599.4500000000007</v>
+      </c>
+      <c r="C133" s="11"/>
       <c r="D133" s="13">
         <f t="shared" si="3"/>
-        <v>12345.78</v>
+        <v>0</v>
       </c>
       <c r="E133" s="11" t="s">
-        <v>78</v>
+        <v>127</v>
       </c>
     </row>
     <row r="134" spans="1:9" ht="15" hidden="1">
       <c r="A134" s="11" t="s">
-        <v>169</v>
+        <v>61</v>
       </c>
       <c r="B134" s="12">
-        <v>8599.4500000000007</v>
+        <v>12310.7</v>
       </c>
       <c r="C134" s="11"/>
       <c r="D134" s="13">
@@ -3320,73 +3295,68 @@
         <v>0</v>
       </c>
       <c r="E134" s="11" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="135" spans="1:9" ht="15" hidden="1">
-      <c r="A135" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="B135" s="12">
-        <v>12310.7</v>
-      </c>
-      <c r="C135" s="11"/>
-      <c r="D135" s="13">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E135" s="11" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="136" spans="1:9" s="2" customFormat="1" ht="15">
-      <c r="A136" s="41" t="s">
+    <row r="135" spans="1:9" s="2" customFormat="1" ht="15">
+      <c r="A135" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="B136" s="41"/>
-      <c r="C136" s="19">
-        <f>SUM(C5:C135)</f>
-        <v>464</v>
-      </c>
-      <c r="D136" s="20">
-        <f>SUBTOTAL(9,D5:D135)</f>
-        <v>1006893.6524999999</v>
-      </c>
-      <c r="E136" s="19"/>
-    </row>
-    <row r="137" spans="1:9" ht="9.75" customHeight="1">
-      <c r="A137" s="3"/>
+      <c r="B135" s="41"/>
+      <c r="C135" s="19">
+        <f>SUM(C5:C134)</f>
+        <v>177</v>
+      </c>
+      <c r="D135" s="20">
+        <f>SUBTOTAL(9,D5:D134)</f>
+        <v>505207.07249999995</v>
+      </c>
+      <c r="E135" s="19"/>
+    </row>
+    <row r="136" spans="1:9" ht="9.75" customHeight="1">
+      <c r="A136" s="3"/>
+    </row>
+    <row r="137" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A137" s="21"/>
+      <c r="B137" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="C137" s="42"/>
+      <c r="D137" s="42"/>
+      <c r="E137" s="22"/>
     </row>
     <row r="138" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A138" s="21"/>
-      <c r="B138" s="42" t="s">
-        <v>74</v>
-      </c>
-      <c r="C138" s="42"/>
-      <c r="D138" s="42"/>
+      <c r="A138" s="23"/>
+      <c r="B138" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C138" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="D138" s="24" t="s">
+        <v>64</v>
+      </c>
       <c r="E138" s="22"/>
+      <c r="I138" s="25"/>
     </row>
     <row r="139" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A139" s="23"/>
-      <c r="B139" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="C139" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="D139" s="24" t="s">
-        <v>64</v>
-      </c>
+      <c r="A139" s="26"/>
+      <c r="B139" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C139" s="27">
+        <v>0</v>
+      </c>
+      <c r="D139" s="11"/>
       <c r="E139" s="22"/>
-      <c r="I139" s="25"/>
     </row>
     <row r="140" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
       <c r="A140" s="26"/>
       <c r="B140" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="C140" s="27">
-        <v>0</v>
+        <v>70</v>
+      </c>
+      <c r="C140" s="32">
+        <v>225000</v>
       </c>
       <c r="D140" s="11"/>
       <c r="E140" s="22"/>
@@ -3396,8 +3366,8 @@
       <c r="B141" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C141" s="32">
-        <v>1000000</v>
+      <c r="C141" s="27">
+        <v>0</v>
       </c>
       <c r="D141" s="11"/>
       <c r="E141" s="22"/>
@@ -3405,27 +3375,27 @@
     <row r="142" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
       <c r="A142" s="26"/>
       <c r="B142" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="C142" s="27">
-        <v>0</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="C142" s="27"/>
       <c r="D142" s="11"/>
       <c r="E142" s="22"/>
     </row>
     <row r="143" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
       <c r="A143" s="26"/>
       <c r="B143" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="C143" s="27"/>
+        <v>72</v>
+      </c>
+      <c r="C143" s="27">
+        <v>0</v>
+      </c>
       <c r="D143" s="11"/>
       <c r="E143" s="22"/>
     </row>
     <row r="144" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
       <c r="A144" s="26"/>
       <c r="B144" s="11" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C144" s="27">
         <v>0</v>
@@ -3434,35 +3404,24 @@
       <c r="E144" s="22"/>
     </row>
     <row r="145" spans="1:5" s="6" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A145" s="26"/>
-      <c r="B145" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="C145" s="27">
-        <v>0</v>
-      </c>
-      <c r="D145" s="11"/>
+      <c r="A145" s="23"/>
+      <c r="B145" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="C145" s="29">
+        <f>SUM(C139:C144)</f>
+        <v>225000</v>
+      </c>
+      <c r="D145" s="30"/>
       <c r="E145" s="22"/>
     </row>
-    <row r="146" spans="1:5" s="6" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A146" s="23"/>
-      <c r="B146" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="C146" s="29">
-        <f>SUM(C140:C145)</f>
-        <v>1000000</v>
-      </c>
-      <c r="D146" s="30"/>
-      <c r="E146" s="22"/>
-    </row>
-    <row r="147" spans="1:5">
-      <c r="A147" s="3"/>
-      <c r="C147" s="4"/>
-      <c r="D147" s="4"/>
+    <row r="146" spans="1:5">
+      <c r="A146" s="3"/>
+      <c r="C146" s="4"/>
+      <c r="D146" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A4:E135">
+  <autoFilter ref="A4:E134">
     <filterColumn colId="2">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -3472,8 +3431,8 @@
   <mergeCells count="4">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A136:B136"/>
-    <mergeCell ref="B138:D138"/>
+    <mergeCell ref="A135:B135"/>
+    <mergeCell ref="B137:D137"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>